<commit_message>
Added code from meeting
</commit_message>
<xml_diff>
--- a/cypress/fixtures/excel/TestExcel.xlsx
+++ b/cypress/fixtures/excel/TestExcel.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sanitarskyi/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sanitarskyi/projects/CypressLearn/cypress/fixtures/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8E58D812-AED1-3E4B-80E0-34BAE973D62E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{601D84DA-07D8-2643-9861-317672D90188}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11580" yWindow="5400" windowWidth="28040" windowHeight="17440" xr2:uid="{19BB2152-3DE0-4748-99E7-7D002A20FAAC}"/>
+    <workbookView xWindow="6520" yWindow="4900" windowWidth="28040" windowHeight="17440" xr2:uid="{19BB2152-3DE0-4748-99E7-7D002A20FAAC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>qwe</t>
   </si>
@@ -47,6 +47,12 @@
   </si>
   <si>
     <t>asdasd</t>
+  </si>
+  <si>
+    <t>gjhg</t>
+  </si>
+  <si>
+    <t>w22w2</t>
   </si>
 </sst>
 </file>
@@ -398,28 +404,45 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{892AB238-A5F3-AB46-8734-6D0AB8F61030}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
+      <c r="C1">
+        <v>123</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
+      </c>
+      <c r="C2">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3">
+        <v>83838</v>
+      </c>
+      <c r="C3" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>